<commit_message>
demonstrate excel update(added countryName)
</commit_message>
<xml_diff>
--- a/COM/COM_Application/COM_WindApplication/bin/Debug/doc/DemonstrateTemplate.xlsx
+++ b/COM/COM_Application/COM_WindApplication/bin/Debug/doc/DemonstrateTemplate.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Регион</t>
   </si>
@@ -36,21 +36,9 @@
     <t>Минск</t>
   </si>
   <si>
-    <t>Гомель</t>
-  </si>
-  <si>
-    <t>Гродно</t>
-  </si>
-  <si>
     <t>Барановичи</t>
   </si>
   <si>
-    <t>Могилев</t>
-  </si>
-  <si>
-    <t>Витебск</t>
-  </si>
-  <si>
     <t>Брест</t>
   </si>
   <si>
@@ -70,18 +58,56 @@
   </si>
   <si>
     <t>&lt;total&gt;</t>
+  </si>
+  <si>
+    <t>Страна</t>
+  </si>
+  <si>
+    <t>&lt;CountyName&gt;</t>
+  </si>
+  <si>
+    <t>Белоарусь</t>
+  </si>
+  <si>
+    <t>Украина</t>
+  </si>
+  <si>
+    <t>Киев</t>
+  </si>
+  <si>
+    <t>Россия</t>
+  </si>
+  <si>
+    <t>Москва</t>
+  </si>
+  <si>
+    <t>Ст. Питербург</t>
+  </si>
+  <si>
+    <t>Польша</t>
+  </si>
+  <si>
+    <t>Катовица</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -155,19 +181,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -228,7 +257,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -263,7 +292,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -440,167 +469,195 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="F2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="6" t="s">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3">
+        <v>-5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3">
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
         <v>-5</v>
       </c>
-      <c r="C3" s="3">
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3">
+        <v>-15</v>
+      </c>
+      <c r="E5" s="3">
+        <v>9</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3">
+        <v>15</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="C7" s="3">
         <v>7</v>
       </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="D7" s="3">
+        <v>-9</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-10</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3">
+        <v>-11</v>
+      </c>
+      <c r="D8" s="3">
+        <v>-8</v>
+      </c>
+      <c r="E8" s="3">
         <v>-5</v>
       </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="C9" s="3">
         <v>-15</v>
       </c>
-      <c r="D5" s="3">
-        <v>9</v>
-      </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3">
-        <v>11</v>
-      </c>
-      <c r="D6" s="3">
-        <v>15</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3">
-        <v>-9</v>
-      </c>
-      <c r="D7" s="3">
-        <v>-10</v>
-      </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3">
-        <v>-11</v>
-      </c>
-      <c r="C8" s="3">
-        <v>-8</v>
-      </c>
-      <c r="D8" s="3">
-        <v>-5</v>
-      </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="3">
-        <v>-15</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="D9" s="3">
         <v>-6</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="3">
         <v>6</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>